<commit_message>
xlsx generation: improve working with formulas
- we now support more types formulas, previously we were throwing a validation error when detecting some type of formulas, the validation was not working correctly and it was preventing some types of formulas to throw error when there was no problem
- cell references in formulas now are updated correctly when the reference points to a cell before or after the origin cell of formula
- cell references that point to non existing cell are also handled better now (though there is still one missing case to handle, support will come later, the case is documented in a test that it is skipped for now)
- added more test cases for different type of formulas
</commit_message>
<xml_diff>
--- a/packages/jsreport-xlsx/test/xlsx/loop-existing-formula-cross-sheet-reference.xlsx
+++ b/packages/jsreport-xlsx/test/xlsx/loop-existing-formula-cross-sheet-reference.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/workspace/jsreport/jsreport/packages/jsreport-xlsx/test/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E013CA8-8E2C-C14F-B4BA-FB4F396EB15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5B68FA-1076-0E4C-A1FF-95CD5FE2EB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45500" yWindow="2020" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{3BEBBF8C-DD02-714E-95D6-F485BE283C4B}"/>
+    <workbookView xWindow="45480" yWindow="2000" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{3BEBBF8C-DD02-714E-95D6-F485BE283C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
     <sheet name="B" sheetId="3" r:id="rId2"/>
     <sheet name="C" sheetId="4" r:id="rId3"/>
-    <sheet name="DATA" sheetId="2" r:id="rId4"/>
+    <sheet name="After Loop" sheetId="5" r:id="rId4"/>
+    <sheet name="DATA" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="2">
   <si>
     <t>{{#each items}}{{value}}</t>
   </si>
@@ -462,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43CFA7EF-B156-8C48-93E9-6490B6EC789D}">
   <dimension ref="A2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,11 +487,56 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07F2964-A0E7-E34F-8259-39F10A99CDFF}">
+  <dimension ref="A2:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="e">
+        <f>A4+DATA!A1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C4" t="e">
+        <f>A4+DATA!B2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D4" t="e">
+        <f>A4+DATA!C3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C8A538-2D5F-804C-A384-4B28BBB128B7}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
xlsx: vertical loop complete support test cases with formulas
</commit_message>
<xml_diff>
--- a/packages/jsreport-xlsx/test/xlsx/loop-existing-formula-cross-sheet-reference.xlsx
+++ b/packages/jsreport-xlsx/test/xlsx/loop-existing-formula-cross-sheet-reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/workspace/jsreport/jsreport/packages/jsreport-xlsx/test/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5B68FA-1076-0E4C-A1FF-95CD5FE2EB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E9BC7B-E176-E345-B0CA-46D474B52402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45480" yWindow="2000" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{3BEBBF8C-DD02-714E-95D6-F485BE283C4B}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="19200" windowHeight="10560" xr2:uid="{3BEBBF8C-DD02-714E-95D6-F485BE283C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -407,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8C395A-A101-4548-A5C3-EF709BD95745}">
   <dimension ref="A2:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07F2964-A0E7-E34F-8259-39F10A99CDFF}">
   <dimension ref="A2:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>